<commit_message>
Adicionado análise de mitigação de ilhas de calor
</commit_message>
<xml_diff>
--- a/dados_areas_verdes_urbanas.xlsx
+++ b/dados_areas_verdes_urbanas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\IdeaProjects\green-areas-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6178C3-89D2-4C75-8376-18E9D1E40DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE14D54-12F4-4B69-83F4-79780BCAAFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="areas_verdes_cau_dgat_sqa" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">areas_verdes_cau_dgat_sqa!$A$1:$I$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">areas_verdes_cau_dgat_sqa!$A$1:$J$72</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="82">
   <si>
     <t>Nome da área</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>Praça Fausto Sales</t>
+  </si>
+  <si>
+    <t>Mitigação de ilhas de calor</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,9 +1158,10 @@
     <col min="7" max="7" width="59.6640625" customWidth="1"/>
     <col min="8" max="8" width="35.77734375" customWidth="1"/>
     <col min="9" max="9" width="29.109375" customWidth="1"/>
+    <col min="10" max="10" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,8 +1189,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1214,8 +1221,11 @@
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1243,8 +1253,11 @@
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1272,8 +1285,11 @@
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1301,8 +1317,11 @@
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1330,8 +1349,11 @@
       <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1359,8 +1381,11 @@
       <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1388,8 +1413,11 @@
       <c r="I8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1417,8 +1445,11 @@
       <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1446,8 +1477,11 @@
       <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1475,8 +1509,11 @@
       <c r="I11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1504,8 +1541,11 @@
       <c r="I12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1533,8 +1573,11 @@
       <c r="I13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1562,8 +1605,11 @@
       <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1591,8 +1637,11 @@
       <c r="I15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -1620,8 +1669,11 @@
       <c r="I16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1649,8 +1701,11 @@
       <c r="I17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1678,8 +1733,11 @@
       <c r="I18" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1707,8 +1765,11 @@
       <c r="I19" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1736,8 +1797,11 @@
       <c r="I20" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1765,8 +1829,11 @@
       <c r="I21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1794,8 +1861,11 @@
       <c r="I22" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1823,8 +1893,11 @@
       <c r="I23" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1852,8 +1925,11 @@
       <c r="I24" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1881,8 +1957,11 @@
       <c r="I25" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1910,8 +1989,11 @@
       <c r="I26" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -1939,8 +2021,11 @@
       <c r="I27" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -1968,8 +2053,11 @@
       <c r="I28" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1997,8 +2085,11 @@
       <c r="I29" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -2026,8 +2117,11 @@
       <c r="I30" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -2055,8 +2149,11 @@
       <c r="I31" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -2084,8 +2181,11 @@
       <c r="I32" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -2113,8 +2213,11 @@
       <c r="I33" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
@@ -2142,8 +2245,11 @@
       <c r="I34" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -2171,8 +2277,11 @@
       <c r="I35" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
@@ -2200,8 +2309,11 @@
       <c r="I36" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
@@ -2229,8 +2341,11 @@
       <c r="I37" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -2258,8 +2373,11 @@
       <c r="I38" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>52</v>
       </c>
@@ -2287,8 +2405,11 @@
       <c r="I39" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>53</v>
       </c>
@@ -2316,8 +2437,11 @@
       <c r="I40" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>54</v>
       </c>
@@ -2345,8 +2469,11 @@
       <c r="I41" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -2374,8 +2501,11 @@
       <c r="I42" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
@@ -2403,8 +2533,11 @@
       <c r="I43" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>56</v>
       </c>
@@ -2432,8 +2565,11 @@
       <c r="I44" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>57</v>
       </c>
@@ -2461,8 +2597,11 @@
       <c r="I45" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
@@ -2490,8 +2629,11 @@
       <c r="I46" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
@@ -2519,8 +2661,11 @@
       <c r="I47" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
@@ -2548,8 +2693,11 @@
       <c r="I48" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
@@ -2577,8 +2725,11 @@
       <c r="I49" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>60</v>
       </c>
@@ -2606,8 +2757,11 @@
       <c r="I50" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>61</v>
       </c>
@@ -2635,8 +2789,11 @@
       <c r="I51" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
@@ -2664,8 +2821,11 @@
       <c r="I52" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J52" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
@@ -2693,8 +2853,11 @@
       <c r="I53" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>64</v>
       </c>
@@ -2722,8 +2885,11 @@
       <c r="I54" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J54" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>65</v>
       </c>
@@ -2751,8 +2917,11 @@
       <c r="I55" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J55" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
@@ -2780,8 +2949,11 @@
       <c r="I56" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J56" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>67</v>
       </c>
@@ -2809,8 +2981,11 @@
       <c r="I57" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>68</v>
       </c>
@@ -2838,8 +3013,11 @@
       <c r="I58" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
@@ -2867,8 +3045,11 @@
       <c r="I59" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>70</v>
       </c>
@@ -2896,8 +3077,11 @@
       <c r="I60" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>71</v>
       </c>
@@ -2925,8 +3109,11 @@
       <c r="I61" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J61" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>72</v>
       </c>
@@ -2954,8 +3141,11 @@
       <c r="I62" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J62" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
@@ -2983,8 +3173,11 @@
       <c r="I63" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>74</v>
       </c>
@@ -3012,8 +3205,11 @@
       <c r="I64" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3041,8 +3237,11 @@
       <c r="I65" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J65" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3070,8 +3269,11 @@
       <c r="I66" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>39</v>
       </c>
@@ -3099,8 +3301,11 @@
       <c r="I67" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>39</v>
       </c>
@@ -3128,8 +3333,11 @@
       <c r="I68" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>77</v>
       </c>
@@ -3157,8 +3365,11 @@
       <c r="I69" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>78</v>
       </c>
@@ -3186,8 +3397,11 @@
       <c r="I70" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>79</v>
       </c>
@@ -3215,8 +3429,11 @@
       <c r="I71" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>80</v>
       </c>
@@ -3244,9 +3461,12 @@
       <c r="I72" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="J72" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I72" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J72" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>